<commit_message>
Working version of webscripts
</commit_message>
<xml_diff>
--- a/templates/webscripts/curriculum_report.xlsx
+++ b/templates/webscripts/curriculum_report.xlsx
@@ -1074,17 +1074,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>35
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1095,12 +1098,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1117,12 +1122,14 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>XLIII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1132,12 +1139,14 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>5.14</t>
+          <t>5.14
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1148,37 +1157,44 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>154
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -1193,17 +1209,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>36
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1238,12 +1257,14 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>XLVI</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1253,13 +1274,14 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>5-14
+          <t>5.14
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1270,7 +1292,8 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1287,7 +1310,8 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1298,12 +1322,14 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1344,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>33
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1339,12 +1368,14 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1355,18 +1386,20 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>ΧΧ
+          <t>XX
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>XLIX</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1376,12 +1409,14 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5.14</t>
+          <t>5.14
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1392,7 +1427,8 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1409,7 +1445,8 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1420,7 +1457,8 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -1441,17 +1479,20 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1468,7 +1509,8 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1485,12 +1527,14 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>XLVII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1506,7 +1550,8 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1517,23 +1562,26 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -1544,12 +1592,14 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -1564,33 +1614,38 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>55
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>23
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>165
- ΤΕΛΟΣ</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1601,18 +1656,20 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>ΧΧ
+          <t>XX
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1628,7 +1685,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>2.8
+          <t>7.7
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -1640,7 +1697,8 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1657,7 +1715,8 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -1668,12 +1727,14 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -1688,17 +1749,20 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>35
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1715,7 +1779,8 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1732,12 +1797,14 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>ΧLV</t>
+          <t>L
+ΤΕΛΙΣ</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1747,13 +1814,14 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>5.14
+          <t>5,14
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1764,7 +1832,8 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1775,29 +1844,32 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>13,2
-TEΛOΣ</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>5,3
+          <t>4.6
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>171</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -1812,17 +1884,20 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>26
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>28
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1833,12 +1908,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1855,12 +1932,14 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>XLIII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1876,7 +1955,8 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1887,33 +1967,38 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>176</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>1.3.4</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -1934,17 +2019,20 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>35
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>29
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>12
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1961,7 +2049,8 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1978,12 +2067,14 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>XLVI</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1999,7 +2090,8 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -2010,7 +2102,8 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -2021,27 +2114,32 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>1.3.4</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>173</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -2056,17 +2154,20 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>40
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>40
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2077,12 +2178,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2093,18 +2196,20 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>ΧΧ
+          <t>VV
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>XLVIII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -2120,7 +2225,8 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -2131,7 +2237,8 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -2148,7 +2255,8 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2159,12 +2267,14 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>183</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -2179,17 +2289,20 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>39
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2224,12 +2337,14 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -2239,13 +2354,14 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>5.14 
+          <t>5.14
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -2256,7 +2372,8 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>1.1</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -2267,27 +2384,31 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>1.3.4</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>183
+          <t>185
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -2303,17 +2424,20 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>26
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2324,7 +2448,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>19
+          <t>21
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -2354,7 +2478,8 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -2370,7 +2495,8 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2381,12 +2507,13 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -2398,7 +2525,8 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -2415,7 +2543,8 @@
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -2430,17 +2559,20 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>28
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2481,7 +2613,8 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -2497,7 +2630,8 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2508,23 +2642,26 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -2541,7 +2678,7 @@
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>183
+          <t>185
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -2557,17 +2694,20 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2578,12 +2718,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2594,18 +2736,20 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>ΚΕΙΜΕΝΟ ΧΧ
+          <t>ΚΕΙΜΕΝΟ XX
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>ΚΕΙΜΕΝΟ XLV</t>
+          <t>ΚΕΙΜΕΝΟ L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -2615,24 +2759,26 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>5.14
+          <t>Παράγραφος 5.14 Αυτεπαγωγή
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>Παράγραφος  7.7. Κυματοσυνάρτηση και Εξίσωση Schrodinger
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>1.2
+          <t>Παράγραφος 1.2
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>Παράγραφος 7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2643,27 +2789,32 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>Ενότητα 6.5 
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>1.3.4</t>
+          <t>Ενότητα 4.6 
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -2678,17 +2829,20 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>36
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>35
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2699,13 +2853,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>19
+          <t>21
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2716,18 +2871,20 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>XX
+          <t>XX 
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>XLVI</t>
+          <t>L 
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -2743,7 +2900,8 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2754,7 +2912,8 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2765,12 +2924,14 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -2803,17 +2964,20 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>40
+TΕΛΟΣ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>11
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2837,23 +3001,25 @@
       <c r="I22" t="inlineStr">
         <is>
           <t>21
+ΤΕΛΟΣ</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>XX
+ΤΕΛΟΣ</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>L
 TΕΛΟΣ</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>ΧΧ
-ΤΕΛΟΣ</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>XLVI</t>
-        </is>
-      </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2869,7 +3035,8 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2880,7 +3047,8 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>5.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2891,23 +3059,25 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>13.2
+          <t>6.5
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>5.3
+          <t>4.6
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -2929,17 +3099,20 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>22
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2956,7 +3129,8 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2967,19 +3141,20 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>ΧΧ
+          <t>XX
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>XLVIII
+          <t>L
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2995,7 +3170,8 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -3006,7 +3182,8 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -3017,12 +3194,14 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -3033,12 +3212,14 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -3053,17 +3234,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3080,7 +3261,8 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -3091,18 +3273,20 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>ΧΧ
+          <t>XX
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -3118,7 +3302,8 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -3129,7 +3314,8 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -3140,27 +3326,32 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>1.3.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -3175,17 +3366,20 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>32
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3202,7 +3396,8 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -3225,7 +3420,8 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -3241,7 +3437,8 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -3252,7 +3449,8 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -3263,22 +3461,26 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>1.3.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -3299,17 +3501,20 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>29
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>23
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3326,7 +3531,8 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -3343,12 +3549,14 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>XLII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -3364,7 +3572,8 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -3375,7 +3584,8 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -3386,22 +3596,26 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>1.3.4</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
@@ -3422,17 +3636,20 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>41
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3449,7 +3666,8 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -3472,7 +3690,8 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -3482,13 +3701,14 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>5,14
+          <t>5.14
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -3499,12 +3719,13 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -3516,22 +3737,26 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>10.6</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>5.2.4</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -3546,17 +3771,20 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>27
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3591,12 +3819,14 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>XLVI</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -3612,7 +3842,8 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -3623,33 +3854,38 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>1.3.2</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -3670,17 +3906,20 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>42
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>23
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3697,7 +3936,8 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -3714,12 +3954,14 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -3729,12 +3971,14 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>5.14</t>
+          <t>5.14
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -3745,38 +3989,44 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>1.3.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -3791,17 +4041,20 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>32
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>27
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3812,12 +4065,14 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -3834,12 +4089,14 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>XLVII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -3855,7 +4112,8 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3872,19 +4130,20 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>142
+          <t>143
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
@@ -3895,12 +4154,14 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -3915,57 +4176,59 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>37</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>22</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>165
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
           <t>21
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>254
+τελος</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
           <t>21
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
           <t>ΧΧ
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
           <t>L
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>236
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
@@ -3976,55 +4239,61 @@
       <c r="N31" t="inlineStr">
         <is>
           <t>5.14
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
           <t>1.2
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
           <t>154
-τέλος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>343
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>236
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>1.3.4</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
         <is>
           <t>185
-τελος</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -4039,17 +4308,20 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>33
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>33
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4078,7 +4350,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>XX
+          <t>ΧΧ
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -4090,7 +4362,8 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -4106,7 +4379,8 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -4117,38 +4391,44 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>4.2.2.</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>179</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -4163,17 +4443,20 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>36
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4184,18 +4467,20 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
           <t>21
-TEΛΟΣ</t>
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -4206,12 +4491,14 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -4227,7 +4514,8 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -4238,38 +4526,44 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>1.3.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -4284,17 +4578,20 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>28
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4305,13 +4602,14 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>19
+          <t>21
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>253</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -4328,12 +4626,14 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>XLIV</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -4349,7 +4649,8 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -4360,7 +4661,8 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -4377,7 +4679,8 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
@@ -4388,12 +4691,14 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W34" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -4408,17 +4713,20 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>28
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4435,7 +4743,8 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -4446,7 +4755,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>XX
+          <t>ΧΧ
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -4458,7 +4767,8 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -4486,7 +4796,8 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -4503,22 +4814,26 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>1.3.2</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
         <is>
-          <t>185</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -4533,17 +4848,20 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>26
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>16
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4560,7 +4878,8 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -4571,7 +4890,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>XX
+          <t>ΧΧ
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -4583,7 +4902,8 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -4599,7 +4919,8 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -4610,7 +4931,8 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -4627,7 +4949,8 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U36" t="inlineStr">
@@ -4644,7 +4967,8 @@
       </c>
       <c r="W36" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -4659,17 +4983,20 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>27
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4686,7 +5013,8 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -4703,12 +5031,14 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>XLIX</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
@@ -4724,7 +5054,8 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -4735,12 +5066,13 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -4752,22 +5084,26 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>1.3.3</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W37" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -4782,32 +5118,38 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>165
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -4824,7 +5166,8 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -4869,17 +5212,20 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W38" t="inlineStr">
@@ -4900,17 +5246,20 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>27
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>31
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4921,12 +5270,14 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>248</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -4937,18 +5288,19 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>XX
-ΤΕΛΟΣ</t>
+          <t>XX</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>XLVII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -4964,7 +5316,8 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -4975,33 +5328,38 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>1.3.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W39" t="inlineStr">
@@ -5022,17 +5380,20 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>31
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -5067,12 +5428,14 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>XLVI</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -5088,7 +5451,8 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -5117,22 +5481,26 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W40" t="inlineStr">
         <is>
-          <t>183</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -5147,17 +5515,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>35</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5168,12 +5536,14 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -5190,12 +5560,14 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t xml:space="preserve">XLVII </t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
@@ -5205,12 +5577,14 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>5.14</t>
+          <t>5.14
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -5221,38 +5595,44 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
         <is>
+          <t>143
+ΤΕΛΟΣ</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
           <t>145
 ΤΕΛΟΣ</t>
         </is>
       </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>1.3.1</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W41" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -5268,17 +5648,20 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>40
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>35
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>18
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5295,7 +5678,8 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -5312,12 +5696,14 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>XLV</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -5327,12 +5713,14 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>5.14</t>
+          <t>5.14
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -5343,22 +5731,26 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>154
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U42" t="inlineStr">
@@ -5369,12 +5761,14 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W42" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -5389,17 +5783,20 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>31
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5410,12 +5807,14 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>248</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -5426,18 +5825,20 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>ΧΧ
+          <t>XX
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>XLVII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -5453,34 +5854,38 @@
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>1.2 
+          <t>1.2
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>145
+          <t>154
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U43" t="inlineStr">
@@ -5513,17 +5918,20 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>32
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>30
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5534,12 +5942,14 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>254
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -5550,7 +5960,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>XX
+          <t>ΧΧ
 ΤΕΛΟΣ</t>
         </is>
       </c>
@@ -5562,7 +5972,8 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -5578,7 +5989,8 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -5589,23 +6001,26 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>154
+          <t>145
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>241
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U44" t="inlineStr">
@@ -5622,7 +6037,8 @@
       </c>
       <c r="W44" t="inlineStr">
         <is>
-          <t>171</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>
@@ -5637,17 +6053,20 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>25
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5658,7 +6077,8 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -5675,13 +6095,14 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>ΧΧ
+          <t>XX
 ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>XLII</t>
+          <t>L
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -5702,7 +6123,8 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>7.7
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -5713,7 +6135,8 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>7.4
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -5724,27 +6147,32 @@
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>143
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>245
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>6.5
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.6
+ΤΕΛΟΣ</t>
         </is>
       </c>
       <c r="W45" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>185
+ΤΕΛΟΣ</t>
         </is>
       </c>
     </row>

</xml_diff>